<commit_message>
update A7-A20 / B1-B2 / B5-B7
</commit_message>
<xml_diff>
--- a/sanshainstar/evidence.xlsx
+++ b/sanshainstar/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="3" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,14 @@
     <sheet name="B2" sheetId="24" r:id="rId24"/>
     <sheet name="B5" sheetId="25" r:id="rId25"/>
     <sheet name="B6" sheetId="26" r:id="rId26"/>
+    <sheet name="B7" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="123">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -104,18 +105,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
     <t>A5</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -140,15 +135,6 @@
     <t>A13</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>A14</t>
   </si>
   <si>
@@ -173,12 +159,6 @@
     <t>B1</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
@@ -261,17 +241,193 @@
   </si>
   <si>
     <t>7B41E7A2E182951617817CF405DD52C4E7CD4B65B4B5BCA6EE5AD4F3E9488FE6</t>
+  </si>
+  <si>
+    <t>B9360BD8666AB0DEA9EDF6F3819312A023AC3CE0AAA7414D4A079D2B15A797A4</t>
+  </si>
+  <si>
+    <t>9865507F3D981EF04ECA3B0ABFECB29F502F117F97798AB3CB12644D8C7B9752</t>
+  </si>
+  <si>
+    <t>35E076B28477E6AF6AE9EFA99FC5B5FE0F8F3AD1516E0DBE2D5FFCF1288C6CA8</t>
+  </si>
+  <si>
+    <t>7C781D62E2449C70528DE7D3B9E4F66622114B95A487AE699A4873FEE4188D20</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>ibc/9BB2196A118D7ACEBB665F7940997E6DAF5E5F9E75A76070780B88B8404D8D13</t>
+  </si>
+  <si>
+    <t>nftA7</t>
+  </si>
+  <si>
+    <t>nftA8</t>
+  </si>
+  <si>
+    <t>nftA9</t>
+  </si>
+  <si>
+    <t>nftA10</t>
+  </si>
+  <si>
+    <t>nftA11</t>
+  </si>
+  <si>
+    <t>nftA12</t>
+  </si>
+  <si>
+    <t>ibc/07F2DC891D69DED571E2A431BD459C3969916B7F650CDEBA0F1F9116DA102721</t>
+  </si>
+  <si>
+    <t>ibc/9235D944440975C7E4AE668C01CAE63699A1C054147D983375D7871A5AEEF44C</t>
+  </si>
+  <si>
+    <t>ibc/5A005EFCE63E9030DBCF654708FD8B920804E457921875C092223A95B1AA8562</t>
+  </si>
+  <si>
+    <t>ibc/B00CD93A23236E4B6891E9513BC294E85B81133CA88C7BABDE2F17D473DDD083</t>
+  </si>
+  <si>
+    <t>ibc/7E906F9BA74C36F31EAF6DBFC7941D3DDA2F518D7F29C60825EEC70B3B03A683</t>
+  </si>
+  <si>
+    <t>50F3513EA781C6ECF3EBC41E3D620DB3657140248D79A079CF092E5E08F90015</t>
+  </si>
+  <si>
+    <t>4C06161134EDBA8FF776062676EF47A6CDE9DD9EBDD6F0C0556CE1423178FAAC</t>
+  </si>
+  <si>
+    <t>3C3DA692E333FE54DE11F1D734140B668C789D5D1D7578EEEEA81B951A7333D7</t>
+  </si>
+  <si>
+    <t>EF04101675C42C8B34EDD3A611913F702EBFC9B8CC08B9E8C1253A0C746A19CF</t>
+  </si>
+  <si>
+    <t>6D3E91521DFCDED33AA841E36BA2330C897819C47AA09D9EE5644E0F777A538F</t>
+  </si>
+  <si>
+    <t>E8D9903C23545458462424F774C99E675A98D26654968D00824D4988A858EBE2</t>
+  </si>
+  <si>
+    <t>A3E86BBED4C5422F839212991795D80B95915794426F23B5060D8B400E12FC76</t>
+  </si>
+  <si>
+    <t>5E062A937DD360149E1A1A5695031877718DD5459F8D2E76FD01D29F764DA154</t>
+  </si>
+  <si>
+    <t>05B3A1ECB3E75B9EA842DF9526B67882CC0D7A5054B9580DC84490CC4D2B56A3</t>
+  </si>
+  <si>
+    <t>498A06A38D04615A7B4D200F58491400712CF9A81B0FC8BBD0005598B87CA9BC</t>
+  </si>
+  <si>
+    <t>260BD63A7559FB1B13A4CEF9CE44BFB74C2B12C5D1A51978DD7CE5908EE90B3B</t>
+  </si>
+  <si>
+    <t>63A5056CDE1ED4063551E88998CFB8C880C08F7D55CCB0A836A822D177107A96</t>
+  </si>
+  <si>
+    <t>934670E7E46D7F0D4DDA7FE878576F5600900E686016F5A6FF715961D0116F96</t>
+  </si>
+  <si>
+    <t>5514A3F25A7B8036939BF5E9DB86EB4BA6A499AD9025C8642B52D90AC85E9E3F</t>
+  </si>
+  <si>
+    <t>07A04D178551162374B1DE281F6D94FECAD0F9560EC35012B91B3D10DB6471E8</t>
+  </si>
+  <si>
+    <t>EE12714A2EF3C59382D51FE31FE1B875A2D22611F246119292541376EE83EAF0</t>
+  </si>
+  <si>
+    <t>CA5FC05DAAEDE3EEF3FBDE61954DA2B1C89F3F792BF7B71EA25A034B5736DCF6</t>
+  </si>
+  <si>
+    <t>42191D7DA708E50D143C7001C4ADC39EB3C4865940ADCD5B0656EE65C951F55A</t>
+  </si>
+  <si>
+    <t>89AF2FADC62C4A4F7F0C14ECD790414507A9873A62468FAA9020364F47BFD6AB</t>
+  </si>
+  <si>
+    <t>4F566A96C14F4D5553B14F377B409F3FC9CD2E8B42DC54F337F62AEF6E030253</t>
+  </si>
+  <si>
+    <t>200B4A6EE44B244C9718378A15082D1C4EE3F5649D8E0775A1F0DA0CD3E83380</t>
+  </si>
+  <si>
+    <t>B879CCEE57FD0E006F1C69463B181703EA6D416480E8B19E4327673045902602</t>
+  </si>
+  <si>
+    <t>1D7C2E99DCCCA6819459289EA087AEE594BDBB5D53A100EAA2F891ED54138677</t>
+  </si>
+  <si>
+    <t>B2D37CFF46E41E298134AB890E7DA5B6B12530F5D3662EF4CC9BEE0C39CBC2AB</t>
+  </si>
+  <si>
+    <t>9B6198CEBF7E9A1B230641FEEBD8F18B0866E4A3C2F2BF1DC429DC5B3F51690A</t>
+  </si>
+  <si>
+    <t>7A68C67BEC6D39A1EFCBF85A209972B9459D9903B10C5AB16ECB9470875E67DB</t>
+  </si>
+  <si>
+    <t>14684769523C248429A79D4EF6DFCD51DC1EAC7AC36DB719D09AA26F951974A4</t>
+  </si>
+  <si>
+    <t>BC27DF55DBA77964C8651E22835843B16EE8A8195323CAB44E5B8FAA08B4CA52</t>
+  </si>
+  <si>
+    <t>2C70080C8A3066701D416AD80167044E68EBB2D419C715EE1854E2496BBB3977</t>
+  </si>
+  <si>
+    <t>6F1AA32402B3C60183DEA9D8F70332E50B789D7CB51E11DB88F050C106E7C21D</t>
+  </si>
+  <si>
+    <t>D3744FEEB628AC7D5CF5EE7EDEBA52641F69D41EC83FFEC87B9B728F15D85E12</t>
+  </si>
+  <si>
+    <t>4A338ACB5DFE773CA19EEBCD37B1367D14FED8043CED25C1AB75C407FA2075C8</t>
+  </si>
+  <si>
+    <t>53F9A6192E02DB7B3D3B9BA845ED1A977E720E721FF45795F5E0BE1AE9F43A7D</t>
+  </si>
+  <si>
+    <t>F5B271F1127570F8180230DC48A1CCEB9D1A820605DDF919A41834C2CAA4B314</t>
+  </si>
+  <si>
+    <t>12AE3FE60C669A46C75860A1D0F68C71F8C2EA32B74A6230997172AD6E9C482E</t>
+  </si>
+  <si>
+    <t>B9BBA362A21769A04096B6C2AE26D39D100F4132CD4CBD1DD2CD2FA6B52595D6</t>
+  </si>
+  <si>
+    <t>A2085A9036F22D004A15177AF0B94F0268D4779BE964B098BDED38BED1F6B9AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -313,6 +469,26 @@
     <font>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -425,30 +601,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -460,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -472,18 +651,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="3"/>
+    <cellStyle name="Обычный 3" xfId="4"/>
+    <cellStyle name="Обычный 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1642,20 +1835,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-    </row>
-    <row r="7" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="7" spans="2:4" ht="17.399999999999999">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1666,14 +1859,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1682,14 +1875,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -1698,14 +1891,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -1714,14 +1907,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="15">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1730,340 +1923,340 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="15">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15">
+      <c r="B19" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15">
+      <c r="B21" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="15">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15">
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="15">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15">
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15">
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="15">
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15">
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15">
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="15">
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15">
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="15">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15">
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="15">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15">
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="15">
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15">
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="15">
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15">
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15">
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15">
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="15">
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15">
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="15">
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15">
       <c r="B47" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="15">
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15">
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="15">
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15">
       <c r="B51" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="15">
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15">
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="15">
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15">
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="15">
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15">
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="15">
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2105,16 +2298,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="14" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="14" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2125,67 +2320,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2205,16 +2400,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="15" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="15" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2225,67 +2422,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2305,16 +2502,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="16" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="16" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2325,67 +2524,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2405,16 +2604,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="17" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="17" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2425,67 +2626,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2505,16 +2706,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="18" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="18" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2525,67 +2728,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2605,16 +2808,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="19" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="19" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2625,71 +2830,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>67</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>69</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2709,16 +2922,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="21" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="21" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2729,71 +2944,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>88</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>57</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>57</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2813,16 +3036,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="22" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="22" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2833,71 +3058,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>89</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>90</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>73</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2917,16 +3150,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="23" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="23" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2937,71 +3172,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>96</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>55</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>73</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3021,16 +3264,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="24" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="24" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3041,71 +3286,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>97</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>99</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>55</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3129,7 +3382,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" style="5" customWidth="1"/>
@@ -3142,7 +3395,7 @@
     <col min="10" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3168,31 +3421,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3202,7 +3455,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3212,7 +3465,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -3222,7 +3475,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3232,7 +3485,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -3242,7 +3495,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3252,7 +3505,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3262,7 +3515,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3285,16 +3538,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="25" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="25" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3305,71 +3560,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>101</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>102</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>72</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>103</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3389,16 +3652,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="26" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="26" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3409,71 +3674,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>105</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>106</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>73</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>57</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>73</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>55</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3493,16 +3774,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="27" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="27" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3513,71 +3796,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>111</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>57</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
       <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>113</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>55</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>55</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>57</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3601,13 +3900,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="28" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3616,67 +3915,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3697,17 +3996,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="29" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3716,67 +4015,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3797,15 +4096,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="30" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3814,67 +4115,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3895,15 +4196,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
     <col min="7" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3912,67 +4215,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="20" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3986,6 +4289,101 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KFFFFFFB6</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KFFFFFFPage &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
+  <cols>
+    <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3997,14 +4395,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="6" width="12.6640625" style="35" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4015,60 +4413,60 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4092,7 +4490,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4100,7 +4498,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4113,68 +4511,68 @@
       <c r="D1" s="33"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D2" s="34"/>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4198,7 +4596,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4206,7 +4604,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4221,60 +4619,60 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4298,7 +4696,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4306,7 +4704,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4321,63 +4719,63 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4401,7 +4799,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
     <col min="3" max="3" width="16" style="35" customWidth="1"/>
@@ -4409,7 +4807,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4424,64 +4822,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4505,7 +4903,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="35" customWidth="1"/>
     <col min="2" max="2" width="16" style="35" customWidth="1"/>
@@ -4515,7 +4913,7 @@
     <col min="7" max="16384" width="12.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4530,64 +4928,64 @@
       </c>
       <c r="E1" s="33"/>
     </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E2" s="34"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
       <c r="E6" s="34"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="34"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="34"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -4607,16 +5005,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" style="13" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" style="13" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -4627,67 +5027,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>75</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>

</xml_diff>